<commit_message>
Add validation script for HUD ALO VPN and new SharePoint scripts; remove deprecated files
</commit_message>
<xml_diff>
--- a/Entra/User Lifecycle/Bulk onboarding PS Graph SDK/Create New User.xlsx
+++ b/Entra/User Lifecycle/Bulk onboarding PS Graph SDK/Create New User.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HUD\Git_Repositories\Microsoft-365-and-Azure\Entra\User Lifecycle\Bulk onboarding PS Graph SDK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64FA211A-A887-42DF-A27B-9C7233ABFC27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94FCDE38-5406-4AAF-9DAA-94EE379D5AB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15645" yWindow="4335" windowWidth="38700" windowHeight="15345" xr2:uid="{EC62C7F1-0864-4F6C-8D7F-6E3A57BB67E6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EC62C7F1-0864-4F6C-8D7F-6E3A57BB67E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,28 +42,6 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
   <si>
@@ -172,25 +150,25 @@
     <t>Level 9,7 Waterloo Quay,Pipitea,Wellington</t>
   </si>
   <si>
-    <t>Isabella</t>
-  </si>
-  <si>
-    <t>DaggCourt</t>
-  </si>
-  <si>
-    <t>Isabella Dagg Court</t>
-  </si>
-  <si>
-    <t>Policy Advisor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Operational Policy </t>
-  </si>
-  <si>
-    <t>Policy</t>
-  </si>
-  <si>
-    <t>Rebekah.Hood@hud.govt.nz</t>
+    <t>Duncan</t>
+  </si>
+  <si>
+    <t>Stuart</t>
+  </si>
+  <si>
+    <t>Duncan Stuart</t>
+  </si>
+  <si>
+    <t>SP Assessor</t>
+  </si>
+  <si>
+    <t>Delivery</t>
+  </si>
+  <si>
+    <t>Portfolio Investment</t>
+  </si>
+  <si>
+    <t>Stacey.Beer@hud.govt.nz</t>
   </si>
 </sst>
 </file>
@@ -232,12 +210,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -555,22 +534,23 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" customWidth="1"/>
-    <col min="6" max="6" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" customWidth="1"/>
-    <col min="8" max="8" width="43.42578125" customWidth="1"/>
-    <col min="9" max="9" width="32.5703125" customWidth="1"/>
-    <col min="10" max="10" width="22.42578125" customWidth="1"/>
-    <col min="11" max="11" width="28.42578125" customWidth="1"/>
-    <col min="12" max="12" width="19.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
@@ -626,326 +606,69 @@
         <v>38</v>
       </c>
       <c r="E2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" t="s">
         <v>39</v>
-      </c>
-      <c r="F2" t="s">
-        <v>40</v>
       </c>
       <c r="G2" t="s">
         <v>32</v>
       </c>
       <c r="H2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>41</v>
       </c>
       <c r="J2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K2" t="str">
         <f>IF(ISBLANK(J2), "", IFERROR(VLOOKUP(J2, Sheet2!$A$2:$B$9, 2, FALSE), ""))</f>
-        <v>HUD_SUBSTANTIVE_POSITION</v>
+        <v>ORA_HRX_CONTRACTOR</v>
       </c>
       <c r="L2" s="2">
-        <v>45670</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L3" s="2"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L4" s="2"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K5" t="str">
-        <f>IF(ISBLANK(J5), "", IFERROR(VLOOKUP(J5, Sheet2!$A$2:$B$9, 2, FALSE), ""))</f>
-        <v/>
-      </c>
-      <c r="L5" s="2"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K6" t="str">
-        <f>IF(ISBLANK(J6), "", IFERROR(VLOOKUP(J6, Sheet2!$A$2:$B$9, 2, FALSE), ""))</f>
-        <v/>
-      </c>
-      <c r="L6" s="2"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K7" t="str">
-        <f>IF(ISBLANK(J7), "", IFERROR(VLOOKUP(J7, Sheet2!$A$2:$B$9, 2, FALSE), ""))</f>
-        <v/>
-      </c>
-      <c r="L7" s="2"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H8" t="str" cm="1">
-        <f t="array" ref="H8">IF(G8="Auckland", AucklandAddresses, IF(G8="Wellington", WellingtonAddresses, ""))</f>
-        <v/>
-      </c>
-      <c r="L8" s="2"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H9" t="str" cm="1">
-        <f t="array" ref="H9">IF(G9="Auckland", AucklandAddresses, IF(G9="Wellington", WellingtonAddresses, ""))</f>
-        <v/>
-      </c>
-      <c r="K9" t="str">
-        <f>IF(ISBLANK(J9), "", IFERROR(VLOOKUP(J9, Sheet2!$A$2:$B$9, 2, FALSE), ""))</f>
-        <v/>
-      </c>
-      <c r="L9" s="2"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H10" t="str" cm="1">
-        <f t="array" ref="H10">IF(G10="Auckland", AucklandAddresses, IF(G10="Wellington", WellingtonAddresses, ""))</f>
-        <v/>
-      </c>
-      <c r="K10" t="str">
-        <f>IF(ISBLANK(J10), "", IFERROR(VLOOKUP(J10, Sheet2!$A$2:$B$9, 2, FALSE), ""))</f>
-        <v/>
-      </c>
-      <c r="L10" s="2"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H11" t="str" cm="1">
-        <f t="array" ref="H11">IF(G11="Auckland", AucklandAddresses, IF(G11="Wellington", WellingtonAddresses, ""))</f>
-        <v/>
-      </c>
-      <c r="K11" t="str">
-        <f>IF(ISBLANK(J11), "", IFERROR(VLOOKUP(J11, Sheet2!$A$2:$B$9, 2, FALSE), ""))</f>
-        <v/>
-      </c>
-      <c r="L11" s="2"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H12" t="str" cm="1">
-        <f t="array" ref="H12">IF(G12="Auckland", AucklandAddresses, IF(G12="Wellington", WellingtonAddresses, ""))</f>
-        <v/>
-      </c>
-      <c r="K12" t="str">
-        <f>IF(ISBLANK(J12), "", IFERROR(VLOOKUP(J12, Sheet2!$A$2:$B$9, 2, FALSE), ""))</f>
-        <v/>
-      </c>
-      <c r="L12" s="2"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H13" t="str" cm="1">
-        <f t="array" ref="H13">IF(G13="Auckland", AucklandAddresses, IF(G13="Wellington", WellingtonAddresses, ""))</f>
-        <v/>
-      </c>
-      <c r="K13" t="str">
-        <f>IF(ISBLANK(J13), "", IFERROR(VLOOKUP(J13, Sheet2!$A$2:$B$9, 2, FALSE), ""))</f>
-        <v/>
-      </c>
-      <c r="L13" s="2"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H14" t="str" cm="1">
-        <f t="array" ref="H14">IF(G14="Auckland", AucklandAddresses, IF(G14="Wellington", WellingtonAddresses, ""))</f>
-        <v/>
-      </c>
-      <c r="K14" t="str">
-        <f>IF(ISBLANK(J14), "", IFERROR(VLOOKUP(J14, Sheet2!$A$2:$B$9, 2, FALSE), ""))</f>
-        <v/>
-      </c>
-      <c r="L14" s="2"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H15" t="str" cm="1">
-        <f t="array" ref="H15">IF(G15="Auckland", AucklandAddresses, IF(G15="Wellington", WellingtonAddresses, ""))</f>
-        <v/>
-      </c>
-      <c r="K15" t="str">
-        <f>IF(ISBLANK(J15), "", IFERROR(VLOOKUP(J15, Sheet2!$A$2:$B$9, 2, FALSE), ""))</f>
-        <v/>
-      </c>
-      <c r="L15" s="2"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H16" t="str" cm="1">
-        <f t="array" ref="H16">IF(G16="Auckland", AucklandAddresses, IF(G16="Wellington", WellingtonAddresses, ""))</f>
-        <v/>
-      </c>
-      <c r="K16" t="str">
-        <f>IF(ISBLANK(J16), "", IFERROR(VLOOKUP(J16, Sheet2!$A$2:$B$9, 2, FALSE), ""))</f>
-        <v/>
-      </c>
-      <c r="L16" s="2"/>
-    </row>
-    <row r="17" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H17" t="str" cm="1">
-        <f t="array" ref="H17">IF(G17="Auckland", AucklandAddresses, IF(G17="Wellington", WellingtonAddresses, ""))</f>
-        <v/>
-      </c>
-      <c r="K17" t="str">
-        <f>IF(ISBLANK(J17), "", IFERROR(VLOOKUP(J17, Sheet2!$A$2:$B$9, 2, FALSE), ""))</f>
-        <v/>
-      </c>
-      <c r="L17" s="2"/>
-    </row>
-    <row r="18" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H18" t="str" cm="1">
-        <f t="array" ref="H18">IF(G18="Auckland", AucklandAddresses, IF(G18="Wellington", WellingtonAddresses, ""))</f>
-        <v/>
-      </c>
-      <c r="K18" t="str">
-        <f>IF(ISBLANK(J18), "", IFERROR(VLOOKUP(J18, Sheet2!$A$2:$B$9, 2, FALSE), ""))</f>
-        <v/>
-      </c>
-      <c r="L18" s="2"/>
-    </row>
-    <row r="19" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H19" t="str" cm="1">
-        <f t="array" ref="H19">IF(G19="Auckland", AucklandAddresses, IF(G19="Wellington", WellingtonAddresses, ""))</f>
-        <v/>
-      </c>
-      <c r="K19" t="str">
-        <f>IF(ISBLANK(J19), "", IFERROR(VLOOKUP(J19, Sheet2!$A$2:$B$9, 2, FALSE), ""))</f>
-        <v/>
-      </c>
-      <c r="L19" s="2"/>
-    </row>
-    <row r="20" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H20" t="str" cm="1">
-        <f t="array" ref="H20">IF(G20="Auckland", AucklandAddresses, IF(G20="Wellington", WellingtonAddresses, ""))</f>
-        <v/>
-      </c>
-      <c r="K20" t="str">
-        <f>IF(ISBLANK(J20), "", IFERROR(VLOOKUP(J20, Sheet2!$A$2:$B$9, 2, FALSE), ""))</f>
-        <v/>
-      </c>
-      <c r="L20" s="2"/>
-    </row>
-    <row r="21" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H21" t="str" cm="1">
-        <f t="array" ref="H21">IF(G21="Auckland", AucklandAddresses, IF(G21="Wellington", WellingtonAddresses, ""))</f>
-        <v/>
-      </c>
-      <c r="K21" t="str">
-        <f>IF(ISBLANK(J21), "", IFERROR(VLOOKUP(J21, Sheet2!$A$2:$B$9, 2, FALSE), ""))</f>
-        <v/>
-      </c>
-      <c r="L21" s="2"/>
-    </row>
-    <row r="22" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H22" t="str" cm="1">
-        <f t="array" ref="H22">IF(G22="Auckland", AucklandAddresses, IF(G22="Wellington", WellingtonAddresses, ""))</f>
-        <v/>
-      </c>
-      <c r="K22" t="str">
-        <f>IF(ISBLANK(J22), "", IFERROR(VLOOKUP(J22, Sheet2!$A$2:$B$9, 2, FALSE), ""))</f>
-        <v/>
-      </c>
-      <c r="L22" s="2"/>
-    </row>
-    <row r="23" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H23" t="str" cm="1">
-        <f t="array" ref="H23">IF(G23="Auckland", AucklandAddresses, IF(G23="Wellington", WellingtonAddresses, ""))</f>
-        <v/>
-      </c>
-      <c r="K23" t="str">
-        <f>IF(ISBLANK(J23), "", IFERROR(VLOOKUP(J23, Sheet2!$A$2:$B$9, 2, FALSE), ""))</f>
-        <v/>
-      </c>
-      <c r="L23" s="2"/>
-    </row>
-    <row r="24" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H24" t="str" cm="1">
-        <f t="array" ref="H24">IF(G24="Auckland", AucklandAddresses, IF(G24="Wellington", WellingtonAddresses, ""))</f>
-        <v/>
-      </c>
-      <c r="K24" t="str">
-        <f>IF(ISBLANK(J24), "", IFERROR(VLOOKUP(J24, Sheet2!$A$2:$B$9, 2, FALSE), ""))</f>
-        <v/>
-      </c>
-      <c r="L24" s="2"/>
-    </row>
-    <row r="25" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H25" t="str" cm="1">
-        <f t="array" ref="H25">IF(G25="Auckland", AucklandAddresses, IF(G25="Wellington", WellingtonAddresses, ""))</f>
-        <v/>
-      </c>
-      <c r="K25" t="str">
-        <f>IF(ISBLANK(J25), "", IFERROR(VLOOKUP(J25, Sheet2!$A$2:$B$9, 2, FALSE), ""))</f>
-        <v/>
-      </c>
-      <c r="L25" s="2"/>
-    </row>
-    <row r="26" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H26" t="str" cm="1">
-        <f t="array" ref="H26">IF(G26="Auckland", AucklandAddresses, IF(G26="Wellington", WellingtonAddresses, ""))</f>
-        <v/>
-      </c>
-      <c r="K26" t="str">
-        <f>IF(ISBLANK(J26), "", IFERROR(VLOOKUP(J26, Sheet2!$A$2:$B$9, 2, FALSE), ""))</f>
-        <v/>
-      </c>
-      <c r="L26" s="2"/>
-    </row>
-    <row r="27" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H27" t="str" cm="1">
-        <f t="array" ref="H27">IF(G27="Auckland", AucklandAddresses, IF(G27="Wellington", WellingtonAddresses, ""))</f>
-        <v/>
-      </c>
-      <c r="K27" t="str">
-        <f>IF(ISBLANK(J27), "", IFERROR(VLOOKUP(J27, Sheet2!$A$2:$B$9, 2, FALSE), ""))</f>
-        <v/>
-      </c>
-      <c r="L27" s="2"/>
-    </row>
-    <row r="28" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H28" t="str" cm="1">
-        <f t="array" ref="H28">IF(G28="Auckland", AucklandAddresses, IF(G28="Wellington", WellingtonAddresses, ""))</f>
-        <v/>
-      </c>
-      <c r="K28" t="str">
-        <f>IF(ISBLANK(J28), "", IFERROR(VLOOKUP(J28, Sheet2!$A$2:$B$9, 2, FALSE), ""))</f>
-        <v/>
-      </c>
-      <c r="L28" s="2"/>
-    </row>
-    <row r="29" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H29" t="str" cm="1">
-        <f t="array" ref="H29">IF(G29="Auckland", AucklandAddresses, IF(G29="Wellington", WellingtonAddresses, ""))</f>
-        <v/>
-      </c>
-      <c r="K29" t="str">
-        <f>IF(ISBLANK(J29), "", IFERROR(VLOOKUP(J29, Sheet2!$A$2:$B$9, 2, FALSE), ""))</f>
-        <v/>
-      </c>
-      <c r="L29" s="2"/>
-    </row>
-    <row r="30" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H30" t="str" cm="1">
-        <f t="array" ref="H30">IF(G30="Auckland", AucklandAddresses, IF(G30="Wellington", WellingtonAddresses, ""))</f>
-        <v/>
-      </c>
-      <c r="K30" t="str">
-        <f>IF(ISBLANK(J30), "", IFERROR(VLOOKUP(J30, Sheet2!$A$2:$B$9, 2, FALSE), ""))</f>
-        <v/>
-      </c>
-      <c r="L30" s="2"/>
-    </row>
-    <row r="31" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H31" t="str" cm="1">
-        <f t="array" ref="H31">IF(G31="Auckland", AucklandAddresses, IF(G31="Wellington", WellingtonAddresses, ""))</f>
-        <v/>
-      </c>
-      <c r="K31" t="str">
-        <f>IF(ISBLANK(J31), "", IFERROR(VLOOKUP(J31, Sheet2!$A$2:$B$9, 2, FALSE), ""))</f>
-        <v/>
-      </c>
-      <c r="L31" s="2"/>
-    </row>
-    <row r="32" spans="8:12" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>45719</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25"/>
+    <row r="17" x14ac:dyDescent="0.25"/>
+    <row r="18" x14ac:dyDescent="0.25"/>
+    <row r="19" x14ac:dyDescent="0.25"/>
+    <row r="20" x14ac:dyDescent="0.25"/>
+    <row r="21" x14ac:dyDescent="0.25"/>
+    <row r="22" x14ac:dyDescent="0.25"/>
+    <row r="23" x14ac:dyDescent="0.25"/>
+    <row r="24" x14ac:dyDescent="0.25"/>
+    <row r="25" x14ac:dyDescent="0.25"/>
+    <row r="26" x14ac:dyDescent="0.25"/>
+    <row r="27" x14ac:dyDescent="0.25"/>
+    <row r="28" x14ac:dyDescent="0.25"/>
+    <row r="29" x14ac:dyDescent="0.25"/>
+    <row r="30" x14ac:dyDescent="0.25"/>
+    <row r="31" x14ac:dyDescent="0.25"/>
+    <row r="32" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H31" xr:uid="{0DCBC82E-758B-44E7-85AE-B365DF3118B0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2" xr:uid="{0DCBC82E-758B-44E7-85AE-B365DF3118B0}">
       <formula1>IF(G2="Auckland", AucklandAddresses, IF(G2="Wellington", WellingtonAddresses, ""))</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 [UNCLASSIFIED]</oddFooter>
   </headerFooter>
@@ -956,13 +679,13 @@
           <x14:formula1>
             <xm:f>Sheet2!$E$2:$E$3</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G31</xm:sqref>
+          <xm:sqref>G2</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FE8F0313-0B5E-4F63-8997-A05B0CCABCDD}">
           <x14:formula1>
             <xm:f>Sheet2!$A$2:$A$9</xm:f>
           </x14:formula1>
-          <xm:sqref>J2:J31</xm:sqref>
+          <xm:sqref>J2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>